<commit_message>
updated real time data to 2023 June'
</commit_message>
<xml_diff>
--- a/workingfolder/OtherData/RealTimeData/RealTimeInfQ.xlsx
+++ b/workingfolder/OtherData/RealTimeData/RealTimeInfQ.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C664"/>
+  <dimension ref="A1:C678"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7696,6 +7696,160 @@
         <v>290.455</v>
       </c>
     </row>
+    <row r="665" spans="1:3">
+      <c r="A665" s="2">
+        <v>44682</v>
+      </c>
+      <c r="B665">
+        <v>291.474</v>
+      </c>
+      <c r="C665">
+        <v>292.289</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3">
+      <c r="A666" s="2">
+        <v>44713</v>
+      </c>
+      <c r="B666">
+        <v>295.328</v>
+      </c>
+      <c r="C666">
+        <v>294.354</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3">
+      <c r="A667" s="2">
+        <v>44743</v>
+      </c>
+      <c r="B667">
+        <v>295.271</v>
+      </c>
+      <c r="C667">
+        <v>295.275</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3">
+      <c r="A668" s="2">
+        <v>44774</v>
+      </c>
+      <c r="B668">
+        <v>295.62</v>
+      </c>
+      <c r="C668">
+        <v>296.95</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3">
+      <c r="A669" s="2">
+        <v>44805</v>
+      </c>
+      <c r="B669">
+        <v>296.761</v>
+      </c>
+      <c r="C669">
+        <v>298.66</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3">
+      <c r="A670" s="2">
+        <v>44835</v>
+      </c>
+      <c r="B670">
+        <v>298.062</v>
+      </c>
+      <c r="C670">
+        <v>299.471</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3">
+      <c r="A671" s="2">
+        <v>44866</v>
+      </c>
+      <c r="B671">
+        <v>298.349</v>
+      </c>
+      <c r="C671">
+        <v>300.066</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3">
+      <c r="A672" s="2">
+        <v>44896</v>
+      </c>
+      <c r="B672">
+        <v>298.112</v>
+      </c>
+      <c r="C672">
+        <v>300.974</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3">
+      <c r="A673" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B673">
+        <v>300.536</v>
+      </c>
+      <c r="C673">
+        <v>302.702</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3">
+      <c r="A674" s="2">
+        <v>44958</v>
+      </c>
+      <c r="B674">
+        <v>301.648</v>
+      </c>
+      <c r="C674">
+        <v>304.07</v>
+      </c>
+    </row>
+    <row r="675" spans="1:3">
+      <c r="A675" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B675">
+        <v>301.808</v>
+      </c>
+      <c r="C675">
+        <v>305.24</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3">
+      <c r="A676" s="2">
+        <v>45017</v>
+      </c>
+      <c r="B676">
+        <v>302.918</v>
+      </c>
+      <c r="C676">
+        <v>306.489</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3">
+      <c r="A677" s="2">
+        <v>45047</v>
+      </c>
+      <c r="B677">
+        <v>303.294</v>
+      </c>
+      <c r="C677">
+        <v>307.824</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3">
+      <c r="A678" s="2">
+        <v>45078</v>
+      </c>
+      <c r="B678">
+        <v>303.841</v>
+      </c>
+      <c r="C678">
+        <v>308.309</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>